<commit_message>
fixed flexibility of graphs
</commit_message>
<xml_diff>
--- a/fam.xlsx
+++ b/fam.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="12315" yWindow="1590" windowWidth="6623" windowHeight="8378" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Дано" sheetId="1" state="visible" r:id="rId1"/>
@@ -74,17 +74,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,455 +463,411 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="14.53125" customWidth="1" style="4" min="1" max="1"/>
-    <col width="10.73046875" customWidth="1" style="4" min="2" max="3"/>
-    <col width="7.73046875" customWidth="1" style="4" min="4" max="4"/>
-    <col width="8.33203125" customWidth="1" style="4" min="5" max="5"/>
-    <col width="9.06640625" customWidth="1" style="4" min="6" max="7"/>
-    <col width="7.3984375" customWidth="1" style="4" min="8" max="8"/>
-    <col width="7.53125" customWidth="1" style="4" min="9" max="9"/>
-    <col width="9.53125" customWidth="1" style="4" min="10" max="10"/>
-    <col width="9.06640625" customWidth="1" style="4" min="11" max="11"/>
-    <col width="9.53125" customWidth="1" style="4" min="12" max="12"/>
-    <col width="9.06640625" customWidth="1" style="4" min="13" max="16"/>
-    <col width="9.06640625" customWidth="1" style="4" min="17" max="16384"/>
+    <col width="14.53125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="10.73046875" customWidth="1" style="1" min="2" max="3"/>
+    <col width="7.73046875" customWidth="1" style="1" min="4" max="4"/>
+    <col width="8.33203125" customWidth="1" style="1" min="5" max="5"/>
+    <col width="9.06640625" customWidth="1" style="1" min="6" max="7"/>
+    <col width="7.3984375" customWidth="1" style="1" min="8" max="8"/>
+    <col width="7.53125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="9.53125" customWidth="1" style="1" min="10" max="10"/>
+    <col width="9.06640625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="9.53125" customWidth="1" style="1" min="12" max="12"/>
+    <col width="9.06640625" customWidth="1" style="1" min="13" max="17"/>
+    <col width="9.06640625" customWidth="1" style="1" min="18" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Rzi, мкм</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Rzb, мкм</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>λ, град</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>ϕ, град</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>ϕ1, град</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>γ, град</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>r, мм</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>ρ, мм</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>hz, мм</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>v, м/мин</t>
         </is>
       </c>
-      <c r="K1" s="3" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>t, мм</t>
         </is>
       </c>
-      <c r="L1" s="3" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>s, мм/об</t>
         </is>
       </c>
-      <c r="M1" s="3" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>σb, Мпа</t>
         </is>
       </c>
-      <c r="N1" s="3" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>σ02, МПа</t>
         </is>
       </c>
-      <c r="P1" s="3" t="n"/>
-      <c r="Q1" s="3" t="n"/>
-      <c r="R1" s="3" t="n"/>
-      <c r="S1" s="1" t="n"/>
-      <c r="T1" s="1" t="n"/>
+      <c r="P1" s="4" t="n"/>
+      <c r="Q1" s="4" t="n"/>
+      <c r="R1" s="4" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="B2" s="4" t="n">
+      <c r="A2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G2" s="4" t="n">
+      <c r="F2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>1.2</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="H2" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I2" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J2" s="4" t="n">
+      <c r="I2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J2" s="1" t="n">
         <v>350</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="K2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L2" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M2" s="4" t="n">
+      <c r="L2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="N2" s="4" t="n">
+      <c r="N2" s="1" t="n">
         <v>290</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="B3" s="4" t="n">
+      <c r="A3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>0.6</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4" t="n">
+      <c r="F3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I3" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J3" s="4" t="n">
+      <c r="I3" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J3" s="1" t="n">
         <v>350</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="K3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L3" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M3" s="4" t="n">
+      <c r="L3" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M3" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="N3" s="4" t="n">
+      <c r="N3" s="1" t="n">
         <v>290</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="n">
+      <c r="A4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>0.7</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4" t="n">
+      <c r="F4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I4" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J4" s="4" t="n">
+      <c r="I4" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="K4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L4" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M4" s="4" t="n">
+      <c r="L4" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M4" s="1" t="n">
         <v>315</v>
       </c>
-      <c r="N4" s="4" t="n">
+      <c r="N4" s="1" t="n">
         <v>130</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="B5" s="4" t="n">
+      <c r="A5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="1" t="n">
         <v>-5</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F5" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4" t="n">
+      <c r="F5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>1.2</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I5" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J5" s="4" t="n">
+      <c r="I5" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L5" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M5" s="4" t="n">
+      <c r="L5" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M5" s="1" t="n">
         <v>315</v>
       </c>
-      <c r="N5" s="4" t="n">
+      <c r="N5" s="1" t="n">
         <v>130</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="B6" s="4" t="n">
+      <c r="A6" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="1" t="n">
         <v>-7</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F6" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G6" s="4" t="n">
+      <c r="F6" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H6" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I6" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J6" s="4" t="n">
+      <c r="I6" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L6" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M6" s="4" t="n">
+      <c r="L6" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M6" s="1" t="n">
         <v>315</v>
       </c>
-      <c r="N6" s="4" t="n">
+      <c r="N6" s="1" t="n">
         <v>130</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="n">
+      <c r="A7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>0.6</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="1" t="n">
         <v>-10</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G7" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H7" s="4" t="n">
+      <c r="F7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I7" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J7" s="4" t="n">
+      <c r="I7" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="K7" s="4" t="n">
+      <c r="K7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L7" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M7" s="4" t="n">
+      <c r="L7" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M7" s="1" t="n">
         <v>315</v>
       </c>
-      <c r="N7" s="4" t="n">
+      <c r="N7" s="1" t="n">
         <v>130</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="B8" s="4" t="n">
+      <c r="A8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>0.7</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="C8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="G8" s="4" t="n">
+      <c r="F8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I8" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J8" s="4" t="n">
+      <c r="I8" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J8" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="K8" s="4" t="n">
+      <c r="K8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L8" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M8" s="4" t="n">
+      <c r="L8" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M8" s="1" t="n">
         <v>315</v>
       </c>
-      <c r="N8" s="4" t="n">
+      <c r="N8" s="1" t="n">
         <v>130</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>12</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>